<commit_message>
Found out what was wrong with the program; managed to include stock prices along with the rest of the data
</commit_message>
<xml_diff>
--- a/Stock Info.xlsx
+++ b/Stock Info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Volume</t>
         </is>
       </c>
@@ -453,1700 +458,2200 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Eloxx Pharmaceuticals, Inc.</t>
+          <t>Madrigal Pharmaceuticals, Inc.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4211.06%</t>
+          <t>233.73%</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>140.68K</t>
+          <t>212.92USD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>6.705M</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Shuttle Pharmaceuticals Holdings, Inc.</t>
+          <t>Soleno Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>65.07%</t>
+          <t>152.34%</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>18.757M</t>
+          <t>2.2900USD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>57.555M</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ra Medical Systems, Inc.</t>
+          <t>Viking Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>46.06%</t>
+          <t>62.34%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>23.705M</t>
+          <t>6.53USD</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>62.098M</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anavex Life Sciences Corp.</t>
+          <t>Wag! Group Co.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>35.85%</t>
+          <t>36.74%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>45.683M</t>
+          <t>2.94USD</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>180.411K</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SatixFy Communications Ltd.</t>
+          <t>Terns Pharmaceuticals, Inc.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>33.17%</t>
+          <t>31.30%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>789.166K</t>
+          <t>9.02USD</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1.672M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Spectrum Brands Holdings, Inc.</t>
+          <t>Cerevel Therapeutics Holdings, Inc.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26.62%</t>
+          <t>24.93%</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3.978M</t>
+          <t>31.67USD</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1.123M</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CollPlant Biotechnologies Ltd.</t>
+          <t>Anebulo Pharmaceuticals, Inc.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>26.49%</t>
+          <t>24.57%</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>27.938K</t>
+          <t>2.94USD</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2.622K</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Venus Acquisition Corporation</t>
+          <t>Celcuity Inc.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>24.77%</t>
+          <t>23.78%</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>89.28K</t>
+          <t>12.39USD</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>80.593K</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TOP Ships Inc.</t>
+          <t>Immix Biopharma, Inc.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22.31%</t>
+          <t>21.31%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>31.24M</t>
+          <t>2.29USD</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>751.009K</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Samsara Inc.</t>
+          <t>Summit Therapeutics Inc.</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>20.20%</t>
+          <t>21.05%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4.975M</t>
+          <t>4.37USD</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>11.387M</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tuesday Morning Corp.</t>
+          <t>BeyondSpring, Inc.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>20.00%</t>
+          <t>14.04%</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>89.208K</t>
+          <t>2.60USD</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6.78M</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>eHealth, Inc.</t>
+          <t>Ellomay Capital Ltd</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>19.68%</t>
+          <t>12.89%</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.871M</t>
+          <t>14.45USD</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>706</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OmniAb, Inc.</t>
+          <t>Ideal Power Inc.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>18.51%</t>
+          <t>11.68%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2.22M</t>
+          <t>11.47USD</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>30.302K</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>American Outdoor Brands, Inc.</t>
+          <t>ZeroFox Holdings, Inc.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17.70%</t>
+          <t>11.44%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>519.663K</t>
+          <t>5.94USD</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>39.969K</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Smartsheet Inc.</t>
+          <t>NewAmsterdam Pharma Company N.V.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16.58%</t>
+          <t>11.15%</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>4.572M</t>
+          <t>11.91USD</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>18.504K</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Vision Marine Technologies Inc.</t>
+          <t>Eloxx Pharmaceuticals, Inc.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16.55%</t>
+          <t>10.65%</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>90.722K</t>
+          <t>2.74USD</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1.342K</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ivanhoe Electric Inc.</t>
+          <t>SenesTech, Inc.</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16.11%</t>
+          <t>10.61%</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>329.192K</t>
+          <t>2.92USD</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>29.131K</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GH Research PLC</t>
+          <t>374Water Inc.</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15.38%</t>
+          <t>10.42%</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>35.232K</t>
+          <t>2.86USD</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>12.771K</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fuwei Films (Holdings) Co., Ltd.</t>
+          <t>Afya Limited</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15.26%</t>
+          <t>10.08%</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6.331K</t>
+          <t>15.72USD</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>310.503K</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PLBY Group, Inc.</t>
+          <t>IES Holdings, Inc.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14.82%</t>
+          <t>10.06%</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.255M</t>
+          <t>31.12USD</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>23.801K</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Vivakor, Inc.</t>
+          <t>Fulcrum Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>13.65%</t>
+          <t>9.91%</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.377M</t>
+          <t>5.88USD</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>685.152K</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Peloton Interactive, Inc.</t>
+          <t>Tandy Leather Factory, Inc.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>13.00%</t>
+          <t>9.76%</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>27.053M</t>
+          <t>4.50USD</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1.493K</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Agenus Inc.</t>
+          <t>Heartbeam, Inc.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>12.50%</t>
+          <t>9.74%</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3.468M</t>
+          <t>5.56USD</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>109.934K</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>UiPath, Inc.</t>
+          <t>Starbox Group Holdings Ltd.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>12.46%</t>
+          <t>9.36%</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>18.556M</t>
+          <t>2.57USD</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>315.826K</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>bluebird bio, Inc.</t>
+          <t>Paysign, Inc.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11.56%</t>
+          <t>9.26%</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>5.598M</t>
+          <t>2.59USD</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>24.665K</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Trevi Therapeutics, Inc.</t>
+          <t>CI&amp;T Inc</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11.52%</t>
+          <t>9.20%</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>41.237K</t>
+          <t>5.70USD</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>26.335K</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Motorsport Games Inc.</t>
+          <t>Amyris, Inc.</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11.46%</t>
+          <t>8.84%</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>62.786K</t>
+          <t>2.15USD</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>7.022M</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Tilly's, Inc.</t>
+          <t>Perfect Corp.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11.39%</t>
+          <t>8.40%</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>888.644K</t>
+          <t>7.10USD</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>100.248K</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Marathon Digital Holdings, Inc.</t>
+          <t>Larimar Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>11.27%</t>
+          <t>8.04%</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>21.988M</t>
+          <t>4.84USD</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>117.592K</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ImmunityBio, Inc.</t>
+          <t>Daktronics, Inc.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11.05%</t>
+          <t>7.87%</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2.025M</t>
+          <t>2.74USD</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>279.093K</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Membership Collective Group Inc.</t>
+          <t>Gilat Satellite Networks Ltd.</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>10.25%</t>
+          <t>7.80%</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>677.584K</t>
+          <t>5.53USD</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>197.483K</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Palisade Bio, Inc.</t>
+          <t>Park City Group, Inc.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>10.13%</t>
+          <t>7.78%</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.269M</t>
+          <t>5.40USD</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>30.446K</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Piedmont Lithium Inc.</t>
+          <t>Zymeworks Inc.</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>10.10%</t>
+          <t>7.74%</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>750.392K</t>
+          <t>6.96USD</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>3.973M</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BioRestorative Therapies, Inc.</t>
+          <t>VolitionRX Limited</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>10.06%</t>
+          <t>7.51%</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>104.264K</t>
+          <t>2.29USD</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>210.543K</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Tilray Brands, Inc. - Class 2</t>
+          <t>Duos Technologies Group, Inc.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>9.83%</t>
+          <t>7.24%</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>58.056M</t>
+          <t>2.30USD</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>278</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Intellinetics, Inc.</t>
+          <t>Empire State Realty OP, L.P. Series ES Operating Partnership</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>9.81%</t>
+          <t>7.10%</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>27.173K</t>
+          <t>6.64USD</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>3.011K</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Unisys Corporation New</t>
+          <t>ATN International, Inc.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>9.79%</t>
+          <t>7.03%</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.847M</t>
+          <t>43.38USD</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>9.627K</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ESS Tech, Inc.</t>
+          <t>Mobileye Global Inc.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>9.74%</t>
+          <t>6.88%</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.19M</t>
+          <t>36.14USD</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1.095M</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Digital Brands Group, Inc.</t>
+          <t>Evoke Pharma, Inc.</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>9.65%</t>
+          <t>6.84%</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2.973M</t>
+          <t>2.03USD</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>23.732K</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Madrigal Pharmaceuticals, Inc.</t>
+          <t>Amerant Bancorp Inc.</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>9.63%</t>
+          <t>6.83%</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>586.037K</t>
+          <t>26.92USD</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>85.567K</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Nikola Corporation</t>
+          <t>Security National Financial Corporation</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>9.62%</t>
+          <t>6.74%</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>9.587M</t>
+          <t>6.69USD</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>4.311K</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>FibroGen, Inc</t>
+          <t>Mannatech, Incorporated</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>9.57%</t>
+          <t>6.63%</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>952.895K</t>
+          <t>21.29USD</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>6.197K</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>FaZe Holdings Inc.</t>
+          <t>Kamada Ltd.</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>9.42%</t>
+          <t>6.56%</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>120.068K</t>
+          <t>4.14USD</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>60.594K</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Heartbeam, Inc.</t>
+          <t>The Singing Machine Company, Inc.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>9.39%</t>
+          <t>6.50%</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>279.793K</t>
+          <t>5.08USD</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>6.097K</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SEACOR Marine Holdings Inc.</t>
+          <t>Biote Corp.</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>9.38%</t>
+          <t>6.43%</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>26.647K</t>
+          <t>4.06USD</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>37.273K</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>TG Therapeutics, Inc.</t>
+          <t>ShockWave Medical, Inc.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>9.35%</t>
+          <t>6.41%</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>3.453M</t>
+          <t>217.48USD</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>337.984K</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Monte Rosa Therapeutics, Inc.</t>
+          <t>Integer Holdings Corporation</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>9.34%</t>
+          <t>6.35%</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>260.264K</t>
+          <t>66.79USD</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>163.808K</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Gossamer Bio, Inc.</t>
+          <t>AMCON Distributing Company</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>9.33%</t>
+          <t>5.86%</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2.476M</t>
+          <t>193.50USD</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>342</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Pulse Biosciences, Inc</t>
+          <t>CollPlant Biotechnologies Ltd.</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>9.33%</t>
+          <t>5.80%</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>100.914K</t>
+          <t>8.92USD</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>13.266K</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Arco Platform Limited</t>
+          <t>Apeiron Capital Investment Corp.</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>9.15%</t>
+          <t>5.77%</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>892.6K</t>
+          <t>10.81USD</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2.116K</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Beam Global</t>
+          <t>Comstock Holding Companies, Inc.</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>8.90%</t>
+          <t>5.67%</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>317.092K</t>
+          <t>4.13USD</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>4.011K</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Brooge Energy Limited</t>
+          <t>Consensus Cloud Solutions, Inc.</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8.74%</t>
+          <t>5.65%</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>3.763K</t>
+          <t>55.58USD</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>39.085K</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>SNDL Inc.</t>
+          <t>Manitex International, Inc.</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8.68%</t>
+          <t>5.53%</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>12.219M</t>
+          <t>4.20USD</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>8.869K</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Wrap Technologies, Inc.</t>
+          <t>Pulse Biosciences, Inc</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8.66%</t>
+          <t>5.43%</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>201.814K</t>
+          <t>2.70USD</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>44.324K</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Roivant Sciences Ltd.</t>
+          <t>BIMI International Medical Inc.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8.62%</t>
+          <t>5.33%</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2.618M</t>
+          <t>2.37USD</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>81.567K</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Array Technologies, Inc.</t>
+          <t>Mammoth Energy Services, Inc.</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8.60%</t>
+          <t>5.20%</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>6.248M</t>
+          <t>7.28USD</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>128.538K</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Farfetch Limited</t>
+          <t>Arcos Dorados Holdings Inc.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8.51%</t>
+          <t>5.11%</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>38.922M</t>
+          <t>7.93USD</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>465.802K</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>SCYNEXIS, Inc.</t>
+          <t>Valhi, Inc.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8.49%</t>
+          <t>5.05%</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>131.33K</t>
+          <t>23.09USD</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>12.184K</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Pyxis Tankers Inc.</t>
+          <t>ProKidney Corp.</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8.40%</t>
+          <t>5.00%</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>158.626K</t>
+          <t>8.40USD</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>7.433K</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>FIGS, Inc.</t>
+          <t>Moog Inc.</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8.39%</t>
+          <t>4.92%</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>5.627M</t>
+          <t>86.73USD</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>67.883K</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Generation Bio Co.</t>
+          <t>China Automotive Systems, Inc.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8.32%</t>
+          <t>4.83%</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>483.562K</t>
+          <t>6.51USD</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>193.543K</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Comstock Holding Companies, Inc.</t>
+          <t>Citizens Financial Services, Inc.</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8.32%</t>
+          <t>4.81%</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>25.351K</t>
+          <t>80.00USD</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>636</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Riot Blockchain, Inc</t>
+          <t>SAI.TECH Global Corporation</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8.30%</t>
+          <t>4.72%</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>8.313M</t>
+          <t>3.33USD</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2.864K</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>LAVA Therapeutics N.V.</t>
+          <t>Park-Ohio Holdings Corp.</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8.30%</t>
+          <t>4.71%</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>79.351K</t>
+          <t>12.45USD</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>6.712K</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Backblaze, Inc.</t>
+          <t>Tidewater Inc.</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8.26%</t>
+          <t>4.68%</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>119.963K</t>
+          <t>32.52USD</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>227.283K</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Quotient Technology Inc.</t>
+          <t>Virco Manufacturing Corporation</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8.19%</t>
+          <t>4.66%</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>749.136K</t>
+          <t>4.19USD</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>22.555K</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Atara Biotherapeutics, Inc.</t>
+          <t>Direct Digital Holdings, Inc.</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8.18%</t>
+          <t>4.62%</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>751.038K</t>
+          <t>2.72USD</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>64.788K</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Rocket Pharmaceuticals, Inc.</t>
+          <t>Edify Acquisition Corp.</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8.10%</t>
+          <t>4.58%</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>942.946K</t>
+          <t>10.50USD</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>120</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Warby Parker Inc.</t>
+          <t>Blue Bird Corporation</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8.10%</t>
+          <t>4.50%</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.029M</t>
+          <t>10.69USD</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>61.882K</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Cognition Therapeutics, Inc.</t>
+          <t>MercadoLibre, Inc.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8.08%</t>
+          <t>4.44%</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>396.039K</t>
+          <t>881.43USD</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>371.679K</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Revolution Medicines, Inc.</t>
+          <t>Perdoceo Education Corporation</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7.90%</t>
+          <t>4.38%</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.335M</t>
+          <t>14.07USD</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>142.926K</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Skillsoft Corp.</t>
+          <t>Manitowoc Company, Inc. (The)</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7.89%</t>
+          <t>4.37%</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>414.245K</t>
+          <t>9.55USD</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>114.176K</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Cricut, Inc.</t>
+          <t>Guardant Health, Inc.</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7.85%</t>
+          <t>4.32%</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>173.958K</t>
+          <t>31.36USD</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>1.73M</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Alector, Inc.</t>
+          <t>Superior Industries International, Inc.</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7.82%</t>
+          <t>4.28%</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>576.774K</t>
+          <t>4.63USD</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>49.607K</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Hydrofarm Holdings Group, Inc.</t>
+          <t>Amprius Technologies, Inc.</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7.80%</t>
+          <t>4.25%</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.333M</t>
+          <t>8.72USD</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>143.323K</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Taysha Gene Therapies, Inc.</t>
+          <t>Ebang International Holdings Inc.</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7.80%</t>
+          <t>4.19%</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>311.112K</t>
+          <t>3.23USD</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>37.6K</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ARS Pharmaceuticals, Inc.</t>
+          <t>DZS Inc.</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7.72%</t>
+          <t>4.18%</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>238.428K</t>
+          <t>11.47USD</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>63.508K</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ImmunoPrecise Antibodies Ltd.</t>
+          <t>HighPeak Energy, Inc.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7.71%</t>
+          <t>4.13%</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>61.043K</t>
+          <t>20.87USD</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>39.161K</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>EQRx, Inc.</t>
+          <t>Arbor Rapha Capital Bioholdings Corp. I</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7.69%</t>
+          <t>4.11%</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2.134M</t>
+          <t>11.15USD</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>441</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Rubicon Technologies, Inc.</t>
+          <t>Greenhill &amp; Co., Inc.</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7.66%</t>
+          <t>4.10%</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>88.128K</t>
+          <t>10.41USD</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>125.419K</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Lions Gate Entertainment Corporation</t>
+          <t>Calavo Growers, Inc.</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7.61%</t>
+          <t>4.10%</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>699.278K</t>
+          <t>34.30USD</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>50.884K</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>SemiLEDS Corporation</t>
+          <t>Acrivon Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7.58%</t>
+          <t>4.09%</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14.86K</t>
+          <t>12.48USD</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>515</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>NWTN Inc.</t>
+          <t>Citizens Holding Company</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7.55%</t>
+          <t>4.02%</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>237.07K</t>
+          <t>13.97USD</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>388</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Century Aluminum Company</t>
+          <t>UroGen Pharma Ltd.</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7.49%</t>
+          <t>4.00%</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1.657M</t>
+          <t>8.06USD</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>18.863K</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Direct Digital Holdings, Inc.</t>
+          <t>Northfield Bancorp, Inc.</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7.47%</t>
+          <t>3.99%</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>57.976K</t>
+          <t>15.37USD</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>69.805K</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>FTAI Infrastructure Inc.</t>
+          <t>UNIVERSAL INSURANCE HOLDINGS INC</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7.46%</t>
+          <t>3.91%</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>1.648M</t>
+          <t>9.96USD</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>103.932K</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Inhibrx, Inc.</t>
+          <t>Olympic Steel, Inc.</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7.44%</t>
+          <t>3.84%</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>406.874K</t>
+          <t>33.52USD</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>37.898K</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Traeger, Inc.</t>
+          <t>HireQuest, Inc.</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7.40%</t>
+          <t>3.82%</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>476.431K</t>
+          <t>19.29USD</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>1.385K</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Compass Therapeutics, Inc.</t>
+          <t>Altice USA, Inc.</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>7.39%</t>
+          <t>3.82%</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>299.501K</t>
+          <t>3.95USD</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>7.386M</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Funko, Inc.</t>
+          <t>Alpha Teknova, Inc.</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>7.35%</t>
+          <t>3.81%</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.262M</t>
+          <t>4.90USD</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>6.229K</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Xometry, Inc.</t>
+          <t>NuScale Power Corporation</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>7.33%</t>
+          <t>3.81%</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>427.879K</t>
+          <t>10.08USD</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>315.417K</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Mobileye Global Inc.</t>
+          <t>Hamilton Beach Brands Holding Company</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>7.29%</t>
+          <t>3.79%</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2.061M</t>
+          <t>13.96USD</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>3.28K</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Prelude Therapeutics Incorporated</t>
+          <t>Valens Semiconductor Ltd.</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>7.26%</t>
+          <t>3.78%</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>28.836K</t>
+          <t>4.94USD</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>60.695K</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Eton Pharmaceuticals, Inc.</t>
+          <t>Prime Number Acquisition I Corp.</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>7.26%</t>
+          <t>3.76%</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>161.214K</t>
+          <t>10.49USD</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>1.7K</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Teekay Tankers Ltd.</t>
+          <t>Cato Corporation (The)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>7.26%</t>
+          <t>3.74%</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>604.895K</t>
+          <t>8.87USD</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>251.815K</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Agios Pharmaceuticals, Inc.</t>
+          <t>Insteel Industries, Inc.</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>7.25%</t>
+          <t>3.71%</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>460.555K</t>
+          <t>25.42USD</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>37.965K</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Cyxtera Technologies, Inc.</t>
+          <t>Williams-Sonoma, Inc.</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>7.21%</t>
+          <t>3.68%</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>765.311K</t>
+          <t>115.82USD</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>587.049K</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Kymera Therapeutics, Inc.</t>
+          <t>Altisource Asset Management Corp Com</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>7.17%</t>
+          <t>3.67%</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>700.039K</t>
+          <t>19.75USD</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>728</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>23andMe Holding Co.</t>
+          <t>Employers Holdings Inc</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>7.10%</t>
+          <t>3.63%</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2.893M</t>
+          <t>42.56USD</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>29.185K</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Mersana Therapeutics, Inc.</t>
+          <t>Nabors Industries Ltd.</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>7.09%</t>
+          <t>3.63%</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>847.353K</t>
+          <t>146.18USD</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>54.746K</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add gitignore to excel files
</commit_message>
<xml_diff>
--- a/Stock Info.xlsx
+++ b/Stock Info.xlsx
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>233.73%</t>
+          <t>234.76%</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>212.92USD</t>
+          <t>213.58USD</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.705M</t>
+          <t>6.726M</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>152.34%</t>
+          <t>147.93%</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2.2900USD</t>
+          <t>2.2500USD</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>57.555M</t>
+          <t>59.161M</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>62.34%</t>
+          <t>64.93%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>6.53USD</t>
+          <t>6.63USD</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>62.098M</t>
+          <t>63.114M</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>180.411K</t>
+          <t>181.641K</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31.30%</t>
+          <t>30.42%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9.02USD</t>
+          <t>8.96USD</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.672M</t>
+          <t>1.678M</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.123M</t>
+          <t>1.135M</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>80.593K</t>
+          <t>80.595K</t>
         </is>
       </c>
     </row>
@@ -639,17 +639,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21.31%</t>
+          <t>22.78%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2.29USD</t>
+          <t>2.32USD</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>751.009K</t>
+          <t>805.565K</t>
         </is>
       </c>
     </row>
@@ -661,39 +661,39 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21.05%</t>
+          <t>21.35%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4.37USD</t>
+          <t>4.38USD</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>11.387M</t>
+          <t>11.749M</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BeyondSpring, Inc.</t>
+          <t>374Water Inc.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>14.04%</t>
+          <t>14.61%</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2.60USD</t>
+          <t>2.97USD</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6.78M</t>
+          <t>13.887K</t>
         </is>
       </c>
     </row>
@@ -715,403 +715,403 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>706</t>
+          <t>710</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ideal Power Inc.</t>
+          <t>BeyondSpring, Inc.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11.68%</t>
+          <t>12.72%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11.47USD</t>
+          <t>2.57USD</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>30.302K</t>
+          <t>6.794M</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ZeroFox Holdings, Inc.</t>
+          <t>Ideal Power Inc.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11.44%</t>
+          <t>11.68%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5.94USD</t>
+          <t>11.47USD</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>39.969K</t>
+          <t>30.302K</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NewAmsterdam Pharma Company N.V.</t>
+          <t>ZeroFox Holdings, Inc.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11.15%</t>
+          <t>11.44%</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11.91USD</t>
+          <t>5.94USD</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>18.504K</t>
+          <t>40.471K</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Eloxx Pharmaceuticals, Inc.</t>
+          <t>NewAmsterdam Pharma Company N.V.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10.65%</t>
+          <t>11.06%</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2.74USD</t>
+          <t>11.90USD</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.342K</t>
+          <t>18.615K</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SenesTech, Inc.</t>
+          <t>Eloxx Pharmaceuticals, Inc.</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10.61%</t>
+          <t>10.65%</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2.92USD</t>
+          <t>2.74USD</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>29.131K</t>
+          <t>1.346K</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>374Water Inc.</t>
+          <t>SenesTech, Inc.</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10.42%</t>
+          <t>10.61%</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2.86USD</t>
+          <t>2.92USD</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12.771K</t>
+          <t>30.131K</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Afya Limited</t>
+          <t>IES Holdings, Inc.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10.08%</t>
+          <t>10.47%</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15.72USD</t>
+          <t>31.24USD</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>310.503K</t>
+          <t>24.286K</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IES Holdings, Inc.</t>
+          <t>Heartbeam, Inc.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>10.06%</t>
+          <t>10.26%</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>31.12USD</t>
+          <t>5.59USD</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>23.801K</t>
+          <t>110.05K</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Fulcrum Therapeutics, Inc.</t>
+          <t>Starbox Group Holdings Ltd.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>9.91%</t>
+          <t>10.21%</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5.88USD</t>
+          <t>2.59USD</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>685.152K</t>
+          <t>316.426K</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tandy Leather Factory, Inc.</t>
+          <t>Afya Limited</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>9.76%</t>
+          <t>10.15%</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>4.50USD</t>
+          <t>15.73USD</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.493K</t>
+          <t>313.154K</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Heartbeam, Inc.</t>
+          <t>Fulcrum Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9.74%</t>
+          <t>10.09%</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>5.56USD</t>
+          <t>5.89USD</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>109.934K</t>
+          <t>685.836K</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Starbox Group Holdings Ltd.</t>
+          <t>Tandy Leather Factory, Inc.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>9.36%</t>
+          <t>9.76%</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.57USD</t>
+          <t>4.50USD</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>315.826K</t>
+          <t>1.493K</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Paysign, Inc.</t>
+          <t>Amyris, Inc.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>9.26%</t>
+          <t>9.60%</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2.59USD</t>
+          <t>2.17USD</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>24.665K</t>
+          <t>7.068M</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CI&amp;T Inc</t>
+          <t>Paysign, Inc.</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>9.20%</t>
+          <t>9.28%</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>5.70USD</t>
+          <t>2.59USD</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>26.335K</t>
+          <t>24.8K</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Amyris, Inc.</t>
+          <t>CI&amp;T Inc</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8.84%</t>
+          <t>9.20%</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2.15USD</t>
+          <t>5.70USD</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7.022M</t>
+          <t>27.868K</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Perfect Corp.</t>
+          <t>Park City Group, Inc.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8.40%</t>
+          <t>8.78%</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>7.10USD</t>
+          <t>5.45USD</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>100.248K</t>
+          <t>33.465K</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Larimar Therapeutics, Inc.</t>
+          <t>Perfect Corp.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>8.04%</t>
+          <t>8.40%</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4.84USD</t>
+          <t>7.10USD</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>117.592K</t>
+          <t>100.268K</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Daktronics, Inc.</t>
+          <t>Larimar Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7.87%</t>
+          <t>8.26%</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2.74USD</t>
+          <t>4.85USD</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>279.093K</t>
+          <t>120.022K</t>
         </is>
       </c>
     </row>
@@ -1123,68 +1123,68 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7.80%</t>
+          <t>8.09%</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>5.53USD</t>
+          <t>5.55USD</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>197.483K</t>
+          <t>204.188K</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Park City Group, Inc.</t>
+          <t>Daktronics, Inc.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7.78%</t>
+          <t>7.87%</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>5.40USD</t>
+          <t>2.74USD</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>30.446K</t>
+          <t>286.772K</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Zymeworks Inc.</t>
+          <t>VolitionRX Limited</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7.74%</t>
+          <t>7.51%</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>6.96USD</t>
+          <t>2.29USD</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3.973M</t>
+          <t>210.581K</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>VolitionRX Limited</t>
+          <t>ATN International, Inc.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1194,100 +1194,100 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2.29USD</t>
+          <t>43.57USD</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>210.543K</t>
+          <t>10.132K</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Duos Technologies Group, Inc.</t>
+          <t>Zymeworks Inc.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7.24%</t>
+          <t>7.43%</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2.30USD</t>
+          <t>6.94USD</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>3.991M</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Empire State Realty OP, L.P. Series ES Operating Partnership</t>
+          <t>Duos Technologies Group, Inc.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7.10%</t>
+          <t>7.24%</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>6.64USD</t>
+          <t>2.30USD</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3.011K</t>
+          <t>278</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ATN International, Inc.</t>
+          <t>Mobileye Global Inc.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7.03%</t>
+          <t>7.11%</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>43.38USD</t>
+          <t>36.21USD</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>9.627K</t>
+          <t>1.124M</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mobileye Global Inc.</t>
+          <t>Empire State Realty OP, L.P. Series ES Operating Partnership</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6.88%</t>
+          <t>7.10%</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>36.14USD</t>
+          <t>6.64USD</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.095M</t>
+          <t>3.014K</t>
         </is>
       </c>
     </row>
@@ -1309,51 +1309,51 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>23.732K</t>
+          <t>23.832K</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Amerant Bancorp Inc.</t>
+          <t>Security National Financial Corporation</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6.83%</t>
+          <t>6.74%</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>26.92USD</t>
+          <t>6.69USD</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>85.567K</t>
+          <t>4.311K</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Security National Financial Corporation</t>
+          <t>Integer Holdings Corporation</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6.74%</t>
+          <t>6.64%</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>6.69USD</t>
+          <t>66.97USD</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4.311K</t>
+          <t>165.627K</t>
         </is>
       </c>
     </row>
@@ -1382,22 +1382,22 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Kamada Ltd.</t>
+          <t>Amerant Bancorp Inc.</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6.56%</t>
+          <t>6.63%</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>4.14USD</t>
+          <t>26.87USD</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>60.594K</t>
+          <t>88.596K</t>
         </is>
       </c>
     </row>
@@ -1426,7 +1426,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Biote Corp.</t>
+          <t>Kamada Ltd.</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1436,254 +1436,254 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>4.06USD</t>
+          <t>4.14USD</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>37.273K</t>
+          <t>62.195K</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ShockWave Medical, Inc.</t>
+          <t>Biote Corp.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6.41%</t>
+          <t>6.30%</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>217.48USD</t>
+          <t>4.05USD</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>337.984K</t>
+          <t>37.438K</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Integer Holdings Corporation</t>
+          <t>ShockWave Medical, Inc.</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6.35%</t>
+          <t>6.11%</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>66.79USD</t>
+          <t>216.86USD</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>163.808K</t>
+          <t>341.839K</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AMCON Distributing Company</t>
+          <t>Consensus Cloud Solutions, Inc.</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5.86%</t>
+          <t>5.91%</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>193.50USD</t>
+          <t>55.72USD</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>39.24K</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CollPlant Biotechnologies Ltd.</t>
+          <t>AMCON Distributing Company</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5.80%</t>
+          <t>5.86%</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>8.92USD</t>
+          <t>193.50USD</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13.266K</t>
+          <t>342</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Apeiron Capital Investment Corp.</t>
+          <t>CollPlant Biotechnologies Ltd.</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5.77%</t>
+          <t>5.80%</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10.81USD</t>
+          <t>8.92USD</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2.116K</t>
+          <t>13.266K</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Comstock Holding Companies, Inc.</t>
+          <t>Apeiron Capital Investment Corp.</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5.67%</t>
+          <t>5.77%</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>4.13USD</t>
+          <t>10.81USD</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>4.011K</t>
+          <t>2.117K</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Consensus Cloud Solutions, Inc.</t>
+          <t>Comstock Holding Companies, Inc.</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5.65%</t>
+          <t>5.67%</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>55.58USD</t>
+          <t>4.13USD</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>39.085K</t>
+          <t>4.111K</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Manitex International, Inc.</t>
+          <t>Mammoth Energy Services, Inc.</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5.53%</t>
+          <t>5.63%</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>4.20USD</t>
+          <t>7.31USD</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>8.869K</t>
+          <t>129.862K</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Pulse Biosciences, Inc</t>
+          <t>Manitex International, Inc.</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5.43%</t>
+          <t>5.53%</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2.70USD</t>
+          <t>4.20USD</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>44.324K</t>
+          <t>8.869K</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BIMI International Medical Inc.</t>
+          <t>Pulse Biosciences, Inc</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>5.33%</t>
+          <t>5.43%</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2.37USD</t>
+          <t>2.70USD</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>81.567K</t>
+          <t>44.324K</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Mammoth Energy Services, Inc.</t>
+          <t>Blue Bird Corporation</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5.20%</t>
+          <t>5.28%</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>7.28USD</t>
+          <t>10.77USD</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>128.538K</t>
+          <t>66.862K</t>
         </is>
       </c>
     </row>
@@ -1705,29 +1705,29 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>465.802K</t>
+          <t>468.251K</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Valhi, Inc.</t>
+          <t>urban-gro, Inc.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>5.05%</t>
+          <t>5.01%</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>23.09USD</t>
+          <t>3.67USD</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12.184K</t>
+          <t>13.12K</t>
         </is>
       </c>
     </row>
@@ -1749,124 +1749,124 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>7.433K</t>
+          <t>7.459K</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Moog Inc.</t>
+          <t>China Automotive Systems, Inc.</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4.92%</t>
+          <t>4.83%</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>86.73USD</t>
+          <t>6.51USD</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>67.883K</t>
+          <t>207.723K</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>China Automotive Systems, Inc.</t>
+          <t>Citizens Financial Services, Inc.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>4.83%</t>
+          <t>4.81%</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>6.51USD</t>
+          <t>80.00USD</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>193.543K</t>
+          <t>636</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Citizens Financial Services, Inc.</t>
+          <t>SAI.TECH Global Corporation</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>4.81%</t>
+          <t>4.72%</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>80.00USD</t>
+          <t>3.33USD</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>636</t>
+          <t>2.864K</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SAI.TECH Global Corporation</t>
+          <t>Park-Ohio Holdings Corp.</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>4.72%</t>
+          <t>4.71%</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>3.33USD</t>
+          <t>12.45USD</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2.864K</t>
+          <t>6.722K</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Park-Ohio Holdings Corp.</t>
+          <t>Tidewater Inc.</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4.71%</t>
+          <t>4.70%</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>12.45USD</t>
+          <t>32.52USD</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>6.712K</t>
+          <t>231.566K</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Tidewater Inc.</t>
+          <t>Moog Inc.</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1876,34 +1876,34 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>32.52USD</t>
+          <t>86.53USD</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>227.283K</t>
+          <t>68.763K</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Virco Manufacturing Corporation</t>
+          <t>MercadoLibre, Inc.</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>4.66%</t>
+          <t>4.62%</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>4.19USD</t>
+          <t>883.00USD</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>22.555K</t>
+          <t>373.704K</t>
         </is>
       </c>
     </row>
@@ -1947,51 +1947,51 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>121</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Blue Bird Corporation</t>
+          <t>Cato Corporation (The)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>4.50%</t>
+          <t>4.44%</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10.69USD</t>
+          <t>8.93USD</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>61.882K</t>
+          <t>262.376K</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MercadoLibre, Inc.</t>
+          <t>Valhi, Inc.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>4.44%</t>
+          <t>4.41%</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>881.43USD</t>
+          <t>22.95USD</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>371.679K</t>
+          <t>12.434K</t>
         </is>
       </c>
     </row>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>4.38%</t>
+          <t>4.34%</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2013,491 +2013,491 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>142.926K</t>
+          <t>144.257K</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Manitowoc Company, Inc. (The)</t>
+          <t>Superior Industries International, Inc.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>4.37%</t>
+          <t>4.28%</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>9.55USD</t>
+          <t>4.63USD</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>114.176K</t>
+          <t>50.707K</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Guardant Health, Inc.</t>
+          <t>Ebang International Holdings Inc.</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>4.32%</t>
+          <t>4.19%</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>31.36USD</t>
+          <t>3.23USD</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1.73M</t>
+          <t>37.602K</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Superior Industries International, Inc.</t>
+          <t>DZS Inc.</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>4.28%</t>
+          <t>4.18%</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>4.63USD</t>
+          <t>11.47USD</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>49.607K</t>
+          <t>63.54K</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Amprius Technologies, Inc.</t>
+          <t>Manitowoc Company, Inc. (The)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>4.25%</t>
+          <t>4.15%</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>8.72USD</t>
+          <t>9.53USD</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>143.323K</t>
+          <t>118.927K</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Ebang International Holdings Inc.</t>
+          <t>Williams-Sonoma, Inc.</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>4.19%</t>
+          <t>4.12%</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>3.23USD</t>
+          <t>116.31USD</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>37.6K</t>
+          <t>597.234K</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DZS Inc.</t>
+          <t>Arbor Rapha Capital Bioholdings Corp. I</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>4.18%</t>
+          <t>4.11%</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>11.47USD</t>
+          <t>11.15USD</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>63.508K</t>
+          <t>441</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>HighPeak Energy, Inc.</t>
+          <t>Calavo Growers, Inc.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>4.13%</t>
+          <t>4.10%</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>20.87USD</t>
+          <t>34.30USD</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>39.161K</t>
+          <t>51.259K</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Arbor Rapha Capital Bioholdings Corp. I</t>
+          <t>CPI Card Group Inc.</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>4.11%</t>
+          <t>4.09%</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11.15USD</t>
+          <t>31.96USD</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>441</t>
+          <t>30.58K</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Greenhill &amp; Co., Inc.</t>
+          <t>Acrivon Therapeutics, Inc.</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>4.10%</t>
+          <t>4.09%</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>10.41USD</t>
+          <t>12.48USD</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>125.419K</t>
+          <t>524</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Calavo Growers, Inc.</t>
+          <t>Guardant Health, Inc.</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>4.10%</t>
+          <t>4.07%</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>34.30USD</t>
+          <t>31.28USD</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>50.884K</t>
+          <t>1.793M</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Acrivon Therapeutics, Inc.</t>
+          <t>Citizens Holding Company</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>4.09%</t>
+          <t>4.02%</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>12.48USD</t>
+          <t>13.97USD</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>515</t>
+          <t>389</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Citizens Holding Company</t>
+          <t>UroGen Pharma Ltd.</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>4.02%</t>
+          <t>4.00%</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>13.97USD</t>
+          <t>8.06USD</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>388</t>
+          <t>18.883K</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>UroGen Pharma Ltd.</t>
+          <t>Altice USA, Inc.</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>4.00%</t>
+          <t>3.95%</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>8.06USD</t>
+          <t>3.95USD</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>18.863K</t>
+          <t>7.513M</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Northfield Bancorp, Inc.</t>
+          <t>HireQuest, Inc.</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>3.99%</t>
+          <t>3.82%</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>15.37USD</t>
+          <t>19.29USD</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>69.805K</t>
+          <t>1.388K</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>UNIVERSAL INSURANCE HOLDINGS INC</t>
+          <t>Virco Manufacturing Corporation</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>3.91%</t>
+          <t>3.82%</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>9.96USD</t>
+          <t>4.15USD</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>103.932K</t>
+          <t>23.655K</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Olympic Steel, Inc.</t>
+          <t>Alpha Teknova, Inc.</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>3.84%</t>
+          <t>3.81%</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>33.52USD</t>
+          <t>4.90USD</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>37.898K</t>
+          <t>6.241K</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>HireQuest, Inc.</t>
+          <t>NuScale Power Corporation</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>3.82%</t>
+          <t>3.81%</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>19.29USD</t>
+          <t>10.08USD</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1.385K</t>
+          <t>317.456K</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Altice USA, Inc.</t>
+          <t>Greenhill &amp; Co., Inc.</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>3.82%</t>
+          <t>3.80%</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>3.95USD</t>
+          <t>10.38USD</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>7.386M</t>
+          <t>128.876K</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Alpha Teknova, Inc.</t>
+          <t>Insteel Industries, Inc.</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>3.81%</t>
+          <t>3.79%</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>4.90USD</t>
+          <t>25.44USD</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>6.229K</t>
+          <t>38.516K</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>NuScale Power Corporation</t>
+          <t>Hamilton Beach Brands Holding Company</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>3.81%</t>
+          <t>3.79%</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>10.08USD</t>
+          <t>13.96USD</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>315.417K</t>
+          <t>3.28K</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Hamilton Beach Brands Holding Company</t>
+          <t>Valens Semiconductor Ltd.</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>3.79%</t>
+          <t>3.78%</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>13.96USD</t>
+          <t>4.94USD</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>3.28K</t>
+          <t>60.723K</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Valens Semiconductor Ltd.</t>
+          <t>Amprius Technologies, Inc.</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>3.78%</t>
+          <t>3.77%</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>4.94USD</t>
+          <t>8.68USD</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>60.695K</t>
+          <t>144.198K</t>
         </is>
       </c>
     </row>
@@ -2526,132 +2526,132 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Cato Corporation (The)</t>
+          <t>UNIVERSAL INSURANCE HOLDINGS INC</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>3.74%</t>
+          <t>3.76%</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>8.87USD</t>
+          <t>9.94USD</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>251.815K</t>
+          <t>107.034K</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Insteel Industries, Inc.</t>
+          <t>Olympic Steel, Inc.</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>3.71%</t>
+          <t>3.75%</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>25.42USD</t>
+          <t>33.49USD</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>37.965K</t>
+          <t>39.406K</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Williams-Sonoma, Inc.</t>
+          <t>HCI Group, Inc.</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>3.68%</t>
+          <t>3.72%</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>115.82USD</t>
+          <t>34.27USD</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>587.049K</t>
+          <t>45.846K</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Altisource Asset Management Corp Com</t>
+          <t>HomeStreet, Inc.</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>3.67%</t>
+          <t>3.71%</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>19.75USD</t>
+          <t>26.02USD</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>728</t>
+          <t>50.437K</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Employers Holdings Inc</t>
+          <t>Altisource Asset Management Corp Com</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>3.63%</t>
+          <t>3.67%</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>42.56USD</t>
+          <t>19.75USD</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>29.185K</t>
+          <t>728</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Nabors Industries Ltd.</t>
+          <t>HighPeak Energy, Inc.</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>3.63%</t>
+          <t>3.67%</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>146.18USD</t>
+          <t>20.78USD</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>54.746K</t>
+          <t>40.689K</t>
         </is>
       </c>
     </row>

</xml_diff>